<commit_message>
introducción de excel por áreas, ajustes varios
</commit_message>
<xml_diff>
--- a/resultados/por_vector/R1.xlsx
+++ b/resultados/por_vector/R1.xlsx
@@ -9,15 +9,16 @@
   <sheets>
     <sheet name="R1_0" sheetId="1" r:id="rId1"/>
     <sheet name="R1_0.1" sheetId="2" r:id="rId2"/>
-    <sheet name="R1_0.3" sheetId="3" r:id="rId3"/>
-    <sheet name="R1_0.4" sheetId="4" r:id="rId4"/>
+    <sheet name="R1_0.2" sheetId="3" r:id="rId3"/>
+    <sheet name="R1_0.3" sheetId="4" r:id="rId4"/>
+    <sheet name="R1_0.4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="179">
   <si>
     <t>ID</t>
   </si>
@@ -3960,13 +3961,13 @@
         <v>92</v>
       </c>
       <c r="C2">
-        <v>310.4172625227204</v>
+        <v>354.7625857402519</v>
       </c>
       <c r="D2">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E2">
-        <v>0.1000700394979756</v>
+        <v>0.1143657594262579</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -3977,13 +3978,13 @@
         <v>93</v>
       </c>
       <c r="C3">
-        <v>488.0122684569848</v>
+        <v>557.7283068079827</v>
       </c>
       <c r="D3">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E3">
-        <v>0.1233600274158202</v>
+        <v>0.1409828884752231</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3994,13 +3995,13 @@
         <v>94</v>
       </c>
       <c r="C4">
-        <v>523.3628148150818</v>
+        <v>598.1289312172364</v>
       </c>
       <c r="D4">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E4">
-        <v>0.07807889225944828</v>
+        <v>0.08923301972508375</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4011,13 +4012,13 @@
         <v>95</v>
       </c>
       <c r="C5">
-        <v>378.1763238617006</v>
+        <v>432.2015129848007</v>
       </c>
       <c r="D5">
-        <v>0.3000000000000001</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E5">
-        <v>0.07963283298835556</v>
+        <v>0.09100895198669209</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -4028,13 +4029,13 @@
         <v>96</v>
       </c>
       <c r="C6">
-        <v>338.2535928873897</v>
+        <v>386.5755347284455</v>
       </c>
       <c r="D6">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E6">
-        <v>0.08957987099771975</v>
+        <v>0.1023769954259654</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -4045,13 +4046,13 @@
         <v>97</v>
       </c>
       <c r="C7">
-        <v>710.8225798603158</v>
+        <v>812.368662697504</v>
       </c>
       <c r="D7">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E7">
-        <v>0.1247713849149229</v>
+        <v>0.1425958684741976</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -4062,13 +4063,13 @@
         <v>98</v>
       </c>
       <c r="C8">
-        <v>1956.558725591879</v>
+        <v>2236.067114962148</v>
       </c>
       <c r="D8">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E8">
-        <v>0.08243348327751754</v>
+        <v>0.09420969517430577</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -4079,13 +4080,13 @@
         <v>99</v>
       </c>
       <c r="C9">
-        <v>1339.957434186123</v>
+        <v>1531.379924784141</v>
       </c>
       <c r="D9">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E9">
-        <v>0.1908499407756906</v>
+        <v>0.2181142180293607</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -4096,13 +4097,13 @@
         <v>100</v>
       </c>
       <c r="C10">
-        <v>1315.547167366489</v>
+        <v>1503.482476990274</v>
       </c>
       <c r="D10">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E10">
-        <v>0.1104017428135691</v>
+        <v>0.1261734203583647</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -4113,13 +4114,13 @@
         <v>101</v>
       </c>
       <c r="C11">
-        <v>548.9869799416126</v>
+        <v>627.4136913618431</v>
       </c>
       <c r="D11">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E11">
-        <v>0.08316724434807038</v>
+        <v>0.0950482792549376</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -4130,13 +4131,13 @@
         <v>102</v>
       </c>
       <c r="C12">
-        <v>384.3112338717561</v>
+        <v>439.2128387105785</v>
       </c>
       <c r="D12">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E12">
-        <v>0.0845569271445008</v>
+        <v>0.09663648816514379</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -4147,13 +4148,13 @@
         <v>103</v>
       </c>
       <c r="C13">
-        <v>1239.320500788444</v>
+        <v>1416.366286615365</v>
       </c>
       <c r="D13">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E13">
-        <v>0.08318145518413611</v>
+        <v>0.09506452021044128</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -4164,13 +4165,13 @@
         <v>104</v>
       </c>
       <c r="C14">
-        <v>1986.028981022385</v>
+        <v>2269.747406882726</v>
       </c>
       <c r="D14">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E14">
-        <v>0.088303276022515</v>
+        <v>0.1009180297400172</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -4181,13 +4182,13 @@
         <v>105</v>
       </c>
       <c r="C15">
-        <v>906.1447663272961</v>
+        <v>1035.594018659767</v>
       </c>
       <c r="D15">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E15">
-        <v>0.07876095317925216</v>
+        <v>0.09001251791914533</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -4198,13 +4199,13 @@
         <v>106</v>
       </c>
       <c r="C16">
-        <v>364.323353382228</v>
+        <v>416.3695467225464</v>
       </c>
       <c r="D16">
-        <v>0.3000000000000001</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E16">
-        <v>0.06875322766224344</v>
+        <v>0.07857511732827824</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -4215,13 +4216,13 @@
         <v>107</v>
       </c>
       <c r="C17">
-        <v>284.2268971924078</v>
+        <v>324.8307396484661</v>
       </c>
       <c r="D17">
-        <v>0.3000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E17">
-        <v>0.05655131261289451</v>
+        <v>0.06463007155759375</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -4232,13 +4233,13 @@
         <v>108</v>
       </c>
       <c r="C18">
-        <v>1511.669872535263</v>
+        <v>1727.622711468873</v>
       </c>
       <c r="D18">
-        <v>0.3000000000000001</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E18">
-        <v>0.08720836924744797</v>
+        <v>0.09966670771136914</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -4249,13 +4250,13 @@
         <v>109</v>
       </c>
       <c r="C19">
-        <v>687.4972837379457</v>
+        <v>785.7111814147952</v>
       </c>
       <c r="D19">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E19">
-        <v>0.06355711229896882</v>
+        <v>0.07263669977025008</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -4266,13 +4267,13 @@
         <v>110</v>
       </c>
       <c r="C20">
-        <v>702.1709596353838</v>
+        <v>802.4810967261531</v>
       </c>
       <c r="D20">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E20">
-        <v>0.06919985805020044</v>
+        <v>0.07908555205737194</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -4283,13 +4284,13 @@
         <v>111</v>
       </c>
       <c r="C21">
-        <v>577.739271503595</v>
+        <v>660.2734531469658</v>
       </c>
       <c r="D21">
-        <v>0.3000000000000001</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E21">
-        <v>0.0737570881531463</v>
+        <v>0.08429381503216722</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -4300,13 +4301,13 @@
         <v>112</v>
       </c>
       <c r="C22">
-        <v>516.2335130794531</v>
+        <v>589.9811578050893</v>
       </c>
       <c r="D22">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E22">
-        <v>0.06065485995528765</v>
+        <v>0.06931983994890016</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -4317,13 +4318,13 @@
         <v>113</v>
       </c>
       <c r="C23">
-        <v>698.2708221968434</v>
+        <v>798.0237967963925</v>
       </c>
       <c r="D23">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E23">
-        <v>0.07194959528045784</v>
+        <v>0.08222810889195183</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -4334,13 +4335,13 @@
         <v>114</v>
       </c>
       <c r="C24">
-        <v>832.2555937386651</v>
+        <v>951.149249987046</v>
       </c>
       <c r="D24">
-        <v>0.3000000000000001</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E24">
-        <v>0.1234617406525241</v>
+        <v>0.1410991321743133</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -4351,13 +4352,13 @@
         <v>115</v>
       </c>
       <c r="C25">
-        <v>1363.544382530795</v>
+        <v>1558.336437178052</v>
       </c>
       <c r="D25">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E25">
-        <v>0.09339345085827365</v>
+        <v>0.1067353724094556</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -4368,13 +4369,13 @@
         <v>116</v>
       </c>
       <c r="C26">
-        <v>801.5849061567114</v>
+        <v>916.0970356076704</v>
       </c>
       <c r="D26">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E26">
-        <v>0.1260551826005208</v>
+        <v>0.1440630658291666</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -4385,13 +4386,13 @@
         <v>117</v>
       </c>
       <c r="C27">
-        <v>267.9330841624316</v>
+        <v>306.209239042779</v>
       </c>
       <c r="D27">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E27">
-        <v>0.0976432522457841</v>
+        <v>0.1115922882808961</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -4402,13 +4403,13 @@
         <v>118</v>
       </c>
       <c r="C28">
-        <v>1661.701906189832</v>
+        <v>1899.08789278838</v>
       </c>
       <c r="D28">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E28">
-        <v>0.06401255465117425</v>
+        <v>0.07315720531562774</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -4419,13 +4420,13 @@
         <v>119</v>
       </c>
       <c r="C29">
-        <v>300.8589598045683</v>
+        <v>343.838811205221</v>
       </c>
       <c r="D29">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E29">
-        <v>0.06208397849867278</v>
+        <v>0.07095311828419748</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -4436,13 +4437,13 @@
         <v>120</v>
       </c>
       <c r="C30">
-        <v>515.9184086059431</v>
+        <v>589.6210384067922</v>
       </c>
       <c r="D30">
-        <v>0.3000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E30">
-        <v>0.05533823968743357</v>
+        <v>0.06324370249992407</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -4453,13 +4454,13 @@
         <v>121</v>
       </c>
       <c r="C31">
-        <v>180.9787367995899</v>
+        <v>206.8328420566743</v>
       </c>
       <c r="D31">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E31">
-        <v>0.05092254833978332</v>
+        <v>0.05819719810260952</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -4470,13 +4471,13 @@
         <v>122</v>
       </c>
       <c r="C32">
-        <v>335.1555509967794</v>
+        <v>383.0349154248908</v>
       </c>
       <c r="D32">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E32">
-        <v>0.06697752817681442</v>
+        <v>0.07654574648778792</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -4487,13 +4488,13 @@
         <v>123</v>
       </c>
       <c r="C33">
-        <v>1711.994942758712</v>
+        <v>1956.5656488671</v>
       </c>
       <c r="D33">
-        <v>0.3000000000000001</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E33">
-        <v>0.07045246678019393</v>
+        <v>0.08051710489165022</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -4504,13 +4505,13 @@
         <v>124</v>
       </c>
       <c r="C34">
-        <v>652.2276101177395</v>
+        <v>745.4029829917023</v>
       </c>
       <c r="D34">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E34">
-        <v>0.06395642382013526</v>
+        <v>0.07309305579444031</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -4521,13 +4522,13 @@
         <v>125</v>
       </c>
       <c r="C35">
-        <v>701.4730829733805</v>
+        <v>801.6835233981493</v>
       </c>
       <c r="D35">
-        <v>0.3000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E35">
-        <v>0.06929498004281147</v>
+        <v>0.07919426290607026</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -4538,13 +4539,13 @@
         <v>126</v>
       </c>
       <c r="C36">
-        <v>670.954256706723</v>
+        <v>766.8048648076834</v>
       </c>
       <c r="D36">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E36">
-        <v>0.07023492690324745</v>
+        <v>0.08026848788942567</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -4555,13 +4556,13 @@
         <v>127</v>
       </c>
       <c r="C37">
-        <v>233.9246592477604</v>
+        <v>267.3424677117262</v>
       </c>
       <c r="D37">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E37">
-        <v>0.06454874703304647</v>
+        <v>0.07376999660919598</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -4572,13 +4573,13 @@
         <v>128</v>
       </c>
       <c r="C38">
-        <v>995.5026362111486</v>
+        <v>1137.717298527027</v>
       </c>
       <c r="D38">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E38">
-        <v>0.06506553177850644</v>
+        <v>0.07436060774686451</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -4589,13 +4590,13 @@
         <v>129</v>
       </c>
       <c r="C39">
-        <v>1055.575694333575</v>
+        <v>1206.372222095515</v>
       </c>
       <c r="D39">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E39">
-        <v>0.0626119991893692</v>
+        <v>0.07155657050213624</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -4606,13 +4607,13 @@
         <v>130</v>
       </c>
       <c r="C40">
-        <v>389.2661768138209</v>
+        <v>444.8756306443668</v>
       </c>
       <c r="D40">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E40">
-        <v>0.06501856970332737</v>
+        <v>0.07430693680380271</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -4623,13 +4624,13 @@
         <v>131</v>
       </c>
       <c r="C41">
-        <v>599.7987018177259</v>
+        <v>685.4842306488298</v>
       </c>
       <c r="D41">
-        <v>0.3000000000000001</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E41">
-        <v>0.06019657786207607</v>
+        <v>0.06879608898522981</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -4640,13 +4641,13 @@
         <v>132</v>
       </c>
       <c r="C42">
-        <v>231.2862198866561</v>
+        <v>264.3271084418927</v>
       </c>
       <c r="D42">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E42">
-        <v>0.06037228396936989</v>
+        <v>0.06899689596499417</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -4657,13 +4658,13 @@
         <v>133</v>
       </c>
       <c r="C43">
-        <v>1253.055524988517</v>
+        <v>1432.063457129734</v>
       </c>
       <c r="D43">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E43">
-        <v>0.06524971490254723</v>
+        <v>0.07457110274576828</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -4674,13 +4675,13 @@
         <v>134</v>
       </c>
       <c r="C44">
-        <v>744.0554080132165</v>
+        <v>850.3490377293904</v>
       </c>
       <c r="D44">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E44">
-        <v>0.06186027668882745</v>
+        <v>0.07069745907294565</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -4691,13 +4692,13 @@
         <v>135</v>
       </c>
       <c r="C45">
-        <v>1467.278688557803</v>
+        <v>1676.889929780347</v>
       </c>
       <c r="D45">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E45">
-        <v>0.06583563012329176</v>
+        <v>0.07524072014090488</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -4708,13 +4709,13 @@
         <v>136</v>
       </c>
       <c r="C46">
-        <v>170.9786567297884</v>
+        <v>195.4041791197583</v>
       </c>
       <c r="D46">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E46">
-        <v>0.05624297918743041</v>
+        <v>0.06427769049992048</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -4725,13 +4726,13 @@
         <v>137</v>
       </c>
       <c r="C47">
-        <v>396.708994174616</v>
+        <v>453.3817076281325</v>
       </c>
       <c r="D47">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E47">
-        <v>0.05261392495684562</v>
+        <v>0.0601301999506807</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -4742,13 +4743,13 @@
         <v>138</v>
       </c>
       <c r="C48">
-        <v>177.6992560488625</v>
+        <v>203.0848640558429</v>
       </c>
       <c r="D48">
-        <v>0.3000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E48">
-        <v>0.06417452367239529</v>
+        <v>0.07334231276845177</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -4759,13 +4760,13 @@
         <v>139</v>
       </c>
       <c r="C49">
-        <v>682.2350483073744</v>
+        <v>779.6971980655708</v>
       </c>
       <c r="D49">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E49">
-        <v>0.08875179501852146</v>
+        <v>0.1014306228783102</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -4776,13 +4777,13 @@
         <v>140</v>
       </c>
       <c r="C50">
-        <v>602.0588764809884</v>
+        <v>688.067287406844</v>
       </c>
       <c r="D50">
-        <v>0.3000000000000001</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E50">
-        <v>0.06340799120389556</v>
+        <v>0.07246627566159494</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -4793,13 +4794,13 @@
         <v>141</v>
       </c>
       <c r="C51">
-        <v>1208.777626889244</v>
+        <v>1381.460145016279</v>
       </c>
       <c r="D51">
-        <v>0.3000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E51">
-        <v>0.06295388921875132</v>
+        <v>0.07194730196428724</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -4810,13 +4811,13 @@
         <v>142</v>
       </c>
       <c r="C52">
-        <v>800.8551332905564</v>
+        <v>915.2630094749217</v>
       </c>
       <c r="D52">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E52">
-        <v>0.06244971407443516</v>
+        <v>0.07137110179935446</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -4827,13 +4828,13 @@
         <v>143</v>
       </c>
       <c r="C53">
-        <v>550.5864214181979</v>
+        <v>629.2416244779406</v>
       </c>
       <c r="D53">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E53">
-        <v>0.06988911162962655</v>
+        <v>0.07987327043385892</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -4844,13 +4845,13 @@
         <v>144</v>
       </c>
       <c r="C54">
-        <v>329.7169742633172</v>
+        <v>376.8193991580769</v>
       </c>
       <c r="D54">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E54">
-        <v>0.0541585043139483</v>
+        <v>0.0618954335016552</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -4861,13 +4862,13 @@
         <v>145</v>
       </c>
       <c r="C55">
-        <v>1565.407741369039</v>
+        <v>1789.037418707473</v>
       </c>
       <c r="D55">
-        <v>0.3000000000000001</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E55">
-        <v>0.06375627179444625</v>
+        <v>0.07286431062222429</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -4878,13 +4879,13 @@
         <v>146</v>
       </c>
       <c r="C56">
-        <v>594.6235457991907</v>
+        <v>679.5697666276465</v>
       </c>
       <c r="D56">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E56">
-        <v>0.06825339139109167</v>
+        <v>0.07800387587553334</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -4895,13 +4896,13 @@
         <v>147</v>
       </c>
       <c r="C57">
-        <v>905.9282679681766</v>
+        <v>1035.346591963631</v>
       </c>
       <c r="D57">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E57">
-        <v>0.06190994792374609</v>
+        <v>0.07075422619856697</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -4912,13 +4913,13 @@
         <v>148</v>
       </c>
       <c r="C58">
-        <v>302.9514503856519</v>
+        <v>346.2302290121736</v>
       </c>
       <c r="D58">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E58">
-        <v>0.06686194005421582</v>
+        <v>0.07641364577624665</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -4929,13 +4930,13 @@
         <v>149</v>
       </c>
       <c r="C59">
-        <v>1375.697023803415</v>
+        <v>1572.225170061045</v>
       </c>
       <c r="D59">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E59">
-        <v>0.1048309855828252</v>
+        <v>0.1198068406660859</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -4946,13 +4947,13 @@
         <v>150</v>
       </c>
       <c r="C60">
-        <v>578.5126357005744</v>
+        <v>661.1572979435136</v>
       </c>
       <c r="D60">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E60">
-        <v>0.0682691333137331</v>
+        <v>0.07802186664426641</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -4963,13 +4964,13 @@
         <v>151</v>
       </c>
       <c r="C61">
-        <v>920.9375175289357</v>
+        <v>1052.500020033069</v>
       </c>
       <c r="D61">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E61">
-        <v>0.07882039691278121</v>
+        <v>0.09008045361460711</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -4980,13 +4981,13 @@
         <v>152</v>
       </c>
       <c r="C62">
-        <v>473.9751504631852</v>
+        <v>541.6858862436403</v>
       </c>
       <c r="D62">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E62">
-        <v>0.06757558461123257</v>
+        <v>0.07722923955569437</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -4997,13 +4998,13 @@
         <v>153</v>
       </c>
       <c r="C63">
-        <v>490.0657728079262</v>
+        <v>560.0751689233443</v>
       </c>
       <c r="D63">
-        <v>0.3000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E63">
-        <v>0.09082019510895593</v>
+        <v>0.1037945086959497</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -5014,13 +5015,13 @@
         <v>154</v>
       </c>
       <c r="C64">
-        <v>307.5921787162156</v>
+        <v>351.5339185328179</v>
       </c>
       <c r="D64">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E64">
-        <v>0.0930405864235377</v>
+        <v>0.1063320987697574</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -5031,13 +5032,13 @@
         <v>155</v>
       </c>
       <c r="C65">
-        <v>1704.624898068311</v>
+        <v>1948.142740649499</v>
       </c>
       <c r="D65">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E65">
-        <v>0.07483317520823177</v>
+        <v>0.08552362880940774</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -5048,13 +5049,13 @@
         <v>156</v>
       </c>
       <c r="C66">
-        <v>404.3540994797295</v>
+        <v>462.1189708339766</v>
       </c>
       <c r="D66">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E66">
-        <v>0.07650976338310871</v>
+        <v>0.08743972958069567</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -5065,13 +5066,13 @@
         <v>157</v>
       </c>
       <c r="C67">
-        <v>886.8515171581267</v>
+        <v>1013.544591037859</v>
       </c>
       <c r="D67">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E67">
-        <v>0.05352151582125086</v>
+        <v>0.06116744665285814</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -5082,13 +5083,13 @@
         <v>158</v>
       </c>
       <c r="C68">
-        <v>1505.1492997304</v>
+        <v>1720.170628263314</v>
       </c>
       <c r="D68">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E68">
-        <v>0.05781697459879383</v>
+        <v>0.06607654239862153</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -5099,13 +5100,13 @@
         <v>159</v>
       </c>
       <c r="C69">
-        <v>939.798945015772</v>
+        <v>1074.055937160882</v>
       </c>
       <c r="D69">
-        <v>0.3000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E69">
-        <v>0.08572461415814758</v>
+        <v>0.09797098760931154</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -5116,13 +5117,13 @@
         <v>160</v>
       </c>
       <c r="C70">
-        <v>2647.504007791044</v>
+        <v>3025.718866046908</v>
       </c>
       <c r="D70">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E70">
-        <v>0.06323454685657411</v>
+        <v>0.07226805355037041</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -5133,13 +5134,13 @@
         <v>161</v>
       </c>
       <c r="C71">
-        <v>313.7797239284938</v>
+        <v>358.6053987754215</v>
       </c>
       <c r="D71">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E71">
-        <v>0.05332762133387046</v>
+        <v>0.06094585295299482</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -5150,13 +5151,13 @@
         <v>162</v>
       </c>
       <c r="C72">
-        <v>64.91167408484395</v>
+        <v>74.18477038267881</v>
       </c>
       <c r="D72">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E72">
-        <v>0.06536925889712382</v>
+        <v>0.0747077244538558</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -5167,13 +5168,13 @@
         <v>163</v>
       </c>
       <c r="C73">
-        <v>53.57064232089613</v>
+        <v>61.2235912238813</v>
       </c>
       <c r="D73">
-        <v>0.3000000000000001</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E73">
-        <v>0.05899850475869618</v>
+        <v>0.06742686258136707</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -5184,13 +5185,13 @@
         <v>164</v>
       </c>
       <c r="C74">
-        <v>78.56807063496755</v>
+        <v>89.79208072567721</v>
       </c>
       <c r="D74">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E74">
-        <v>0.06596815334590055</v>
+        <v>0.07539217525245777</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -5201,13 +5202,13 @@
         <v>165</v>
       </c>
       <c r="C75">
-        <v>23.72904097965595</v>
+        <v>27.11890397674965</v>
       </c>
       <c r="D75">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E75">
-        <v>0.06536925889712382</v>
+        <v>0.07470772445385579</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -5218,13 +5219,13 @@
         <v>166</v>
       </c>
       <c r="C76">
-        <v>3.726047757136057</v>
+        <v>4.258340293869781</v>
       </c>
       <c r="D76">
-        <v>0.3</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E76">
-        <v>0.06536925889712381</v>
+        <v>0.0747077244538558</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -5235,13 +5236,13 @@
         <v>167</v>
       </c>
       <c r="C77">
-        <v>236.2103005408986</v>
+        <v>269.9546291895984</v>
       </c>
       <c r="D77">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E77">
-        <v>0.09455976803078406</v>
+        <v>0.1080683063208961</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -5252,13 +5253,13 @@
         <v>168</v>
       </c>
       <c r="C78">
-        <v>47.26385555174958</v>
+        <v>54.01583491628524</v>
       </c>
       <c r="D78">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E78">
-        <v>0.06439217377622558</v>
+        <v>0.07359105574425781</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -5269,13 +5270,13 @@
         <v>169</v>
       </c>
       <c r="C79">
-        <v>792.1290929335046</v>
+        <v>905.2903919240052</v>
       </c>
       <c r="D79">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E79">
-        <v>0.05922460507914053</v>
+        <v>0.06768526294758917</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -5286,13 +5287,13 @@
         <v>170</v>
       </c>
       <c r="C80">
-        <v>80.50909707054494</v>
+        <v>92.01039665205138</v>
       </c>
       <c r="D80">
-        <v>0.3000000000000001</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E80">
-        <v>0.06875243131558065</v>
+        <v>0.07857420721780647</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -5303,13 +5304,13 @@
         <v>171</v>
       </c>
       <c r="C81">
-        <v>75.45474883756356</v>
+        <v>86.23399867150123</v>
       </c>
       <c r="D81">
-        <v>0.3000000000000001</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E81">
-        <v>0.05890300455703634</v>
+        <v>0.06731771949375584</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -5320,13 +5321,13 @@
         <v>172</v>
       </c>
       <c r="C82">
-        <v>428.0835630738745</v>
+        <v>489.2383577987138</v>
       </c>
       <c r="D82">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E82">
-        <v>0.06297198633037283</v>
+        <v>0.07196798437756896</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -5337,13 +5338,13 @@
         <v>173</v>
       </c>
       <c r="C83">
-        <v>174.291592217852</v>
+        <v>199.1903911061166</v>
       </c>
       <c r="D83">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E83">
-        <v>0.0671126654670204</v>
+        <v>0.07670018910516618</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -5354,13 +5355,13 @@
         <v>174</v>
       </c>
       <c r="C84">
-        <v>155.0102027654304</v>
+        <v>177.1545174462061</v>
       </c>
       <c r="D84">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E84">
-        <v>0.08179957929574162</v>
+        <v>0.09348523348084757</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -5371,13 +5372,13 @@
         <v>175</v>
       </c>
       <c r="C85">
-        <v>50.47281390518645</v>
+        <v>57.68321589164166</v>
       </c>
       <c r="D85">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E85">
-        <v>0.06615047693995603</v>
+        <v>0.07560054507423547</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -5388,13 +5389,13 @@
         <v>176</v>
       </c>
       <c r="C86">
-        <v>119.2026560787126</v>
+        <v>136.2316069471001</v>
       </c>
       <c r="D86">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E86">
-        <v>0.08010931188085524</v>
+        <v>0.091553499292406</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -5405,13 +5406,13 @@
         <v>177</v>
       </c>
       <c r="C87">
-        <v>281.4677299644492</v>
+        <v>321.6774056736563</v>
       </c>
       <c r="D87">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E87">
-        <v>0.05770146165732867</v>
+        <v>0.06594452760837562</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -5422,13 +5423,13 @@
         <v>178</v>
       </c>
       <c r="C88">
-        <v>94.3524263595417</v>
+        <v>107.8313444109048</v>
       </c>
       <c r="D88">
-        <v>0.3000000000000001</v>
+        <v>0.1999999999999999</v>
       </c>
       <c r="E88">
-        <v>0.05937849361833965</v>
+        <v>0.06786113556381675</v>
       </c>
     </row>
   </sheetData>
@@ -5469,6 +5470,1515 @@
         <v>92</v>
       </c>
       <c r="C2">
+        <v>310.4172625227204</v>
+      </c>
+      <c r="D2">
+        <v>0.3</v>
+      </c>
+      <c r="E2">
+        <v>0.1000700394979756</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3">
+        <v>488.0122684569848</v>
+      </c>
+      <c r="D3">
+        <v>0.3</v>
+      </c>
+      <c r="E3">
+        <v>0.1233600274158202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4">
+        <v>523.3628148150818</v>
+      </c>
+      <c r="D4">
+        <v>0.3</v>
+      </c>
+      <c r="E4">
+        <v>0.07807889225944828</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5">
+        <v>378.1763238617006</v>
+      </c>
+      <c r="D5">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E5">
+        <v>0.07963283298835556</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6">
+        <v>338.2535928873897</v>
+      </c>
+      <c r="D6">
+        <v>0.3</v>
+      </c>
+      <c r="E6">
+        <v>0.08957987099771975</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7">
+        <v>710.8225798603158</v>
+      </c>
+      <c r="D7">
+        <v>0.3</v>
+      </c>
+      <c r="E7">
+        <v>0.1247713849149229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8">
+        <v>1956.558725591879</v>
+      </c>
+      <c r="D8">
+        <v>0.3</v>
+      </c>
+      <c r="E8">
+        <v>0.08243348327751754</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9">
+        <v>1339.957434186123</v>
+      </c>
+      <c r="D9">
+        <v>0.3</v>
+      </c>
+      <c r="E9">
+        <v>0.1908499407756906</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>1315.547167366489</v>
+      </c>
+      <c r="D10">
+        <v>0.3</v>
+      </c>
+      <c r="E10">
+        <v>0.1104017428135691</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11">
+        <v>548.9869799416126</v>
+      </c>
+      <c r="D11">
+        <v>0.3</v>
+      </c>
+      <c r="E11">
+        <v>0.08316724434807038</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12">
+        <v>384.3112338717561</v>
+      </c>
+      <c r="D12">
+        <v>0.3</v>
+      </c>
+      <c r="E12">
+        <v>0.0845569271445008</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13">
+        <v>1239.320500788444</v>
+      </c>
+      <c r="D13">
+        <v>0.3</v>
+      </c>
+      <c r="E13">
+        <v>0.08318145518413611</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14">
+        <v>1986.028981022385</v>
+      </c>
+      <c r="D14">
+        <v>0.3</v>
+      </c>
+      <c r="E14">
+        <v>0.088303276022515</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15">
+        <v>906.1447663272961</v>
+      </c>
+      <c r="D15">
+        <v>0.3</v>
+      </c>
+      <c r="E15">
+        <v>0.07876095317925216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16">
+        <v>364.323353382228</v>
+      </c>
+      <c r="D16">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E16">
+        <v>0.06875322766224344</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17">
+        <v>284.2268971924078</v>
+      </c>
+      <c r="D17">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E17">
+        <v>0.05655131261289451</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18">
+        <v>1511.669872535263</v>
+      </c>
+      <c r="D18">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E18">
+        <v>0.08720836924744797</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19">
+        <v>687.4972837379457</v>
+      </c>
+      <c r="D19">
+        <v>0.3</v>
+      </c>
+      <c r="E19">
+        <v>0.06355711229896882</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20">
+        <v>702.1709596353838</v>
+      </c>
+      <c r="D20">
+        <v>0.3</v>
+      </c>
+      <c r="E20">
+        <v>0.06919985805020044</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21">
+        <v>577.739271503595</v>
+      </c>
+      <c r="D21">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E21">
+        <v>0.0737570881531463</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22">
+        <v>516.2335130794531</v>
+      </c>
+      <c r="D22">
+        <v>0.3</v>
+      </c>
+      <c r="E22">
+        <v>0.06065485995528765</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23">
+        <v>698.2708221968434</v>
+      </c>
+      <c r="D23">
+        <v>0.3</v>
+      </c>
+      <c r="E23">
+        <v>0.07194959528045784</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24">
+        <v>832.2555937386651</v>
+      </c>
+      <c r="D24">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E24">
+        <v>0.1234617406525241</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25">
+        <v>1363.544382530795</v>
+      </c>
+      <c r="D25">
+        <v>0.3</v>
+      </c>
+      <c r="E25">
+        <v>0.09339345085827365</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26">
+        <v>801.5849061567114</v>
+      </c>
+      <c r="D26">
+        <v>0.3</v>
+      </c>
+      <c r="E26">
+        <v>0.1260551826005208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27">
+        <v>267.9330841624316</v>
+      </c>
+      <c r="D27">
+        <v>0.3</v>
+      </c>
+      <c r="E27">
+        <v>0.0976432522457841</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28">
+        <v>1661.701906189832</v>
+      </c>
+      <c r="D28">
+        <v>0.3</v>
+      </c>
+      <c r="E28">
+        <v>0.06401255465117425</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29">
+        <v>300.8589598045683</v>
+      </c>
+      <c r="D29">
+        <v>0.3</v>
+      </c>
+      <c r="E29">
+        <v>0.06208397849867278</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30">
+        <v>515.9184086059431</v>
+      </c>
+      <c r="D30">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E30">
+        <v>0.05533823968743357</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31">
+        <v>180.9787367995899</v>
+      </c>
+      <c r="D31">
+        <v>0.3</v>
+      </c>
+      <c r="E31">
+        <v>0.05092254833978332</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32">
+        <v>335.1555509967794</v>
+      </c>
+      <c r="D32">
+        <v>0.3</v>
+      </c>
+      <c r="E32">
+        <v>0.06697752817681442</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33">
+        <v>1711.994942758712</v>
+      </c>
+      <c r="D33">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E33">
+        <v>0.07045246678019393</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34">
+        <v>652.2276101177395</v>
+      </c>
+      <c r="D34">
+        <v>0.3</v>
+      </c>
+      <c r="E34">
+        <v>0.06395642382013526</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35">
+        <v>701.4730829733805</v>
+      </c>
+      <c r="D35">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E35">
+        <v>0.06929498004281147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36">
+        <v>670.954256706723</v>
+      </c>
+      <c r="D36">
+        <v>0.3</v>
+      </c>
+      <c r="E36">
+        <v>0.07023492690324745</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37">
+        <v>233.9246592477604</v>
+      </c>
+      <c r="D37">
+        <v>0.3</v>
+      </c>
+      <c r="E37">
+        <v>0.06454874703304647</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" t="s">
+        <v>128</v>
+      </c>
+      <c r="C38">
+        <v>995.5026362111486</v>
+      </c>
+      <c r="D38">
+        <v>0.3</v>
+      </c>
+      <c r="E38">
+        <v>0.06506553177850644</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" t="s">
+        <v>129</v>
+      </c>
+      <c r="C39">
+        <v>1055.575694333575</v>
+      </c>
+      <c r="D39">
+        <v>0.3</v>
+      </c>
+      <c r="E39">
+        <v>0.0626119991893692</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40">
+        <v>389.2661768138209</v>
+      </c>
+      <c r="D40">
+        <v>0.3</v>
+      </c>
+      <c r="E40">
+        <v>0.06501856970332737</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" t="s">
+        <v>131</v>
+      </c>
+      <c r="C41">
+        <v>599.7987018177259</v>
+      </c>
+      <c r="D41">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E41">
+        <v>0.06019657786207607</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" t="s">
+        <v>132</v>
+      </c>
+      <c r="C42">
+        <v>231.2862198866561</v>
+      </c>
+      <c r="D42">
+        <v>0.3</v>
+      </c>
+      <c r="E42">
+        <v>0.06037228396936989</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>133</v>
+      </c>
+      <c r="C43">
+        <v>1253.055524988517</v>
+      </c>
+      <c r="D43">
+        <v>0.3</v>
+      </c>
+      <c r="E43">
+        <v>0.06524971490254723</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44">
+        <v>744.0554080132165</v>
+      </c>
+      <c r="D44">
+        <v>0.3</v>
+      </c>
+      <c r="E44">
+        <v>0.06186027668882745</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45">
+        <v>1467.278688557803</v>
+      </c>
+      <c r="D45">
+        <v>0.3</v>
+      </c>
+      <c r="E45">
+        <v>0.06583563012329176</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" t="s">
+        <v>136</v>
+      </c>
+      <c r="C46">
+        <v>170.9786567297884</v>
+      </c>
+      <c r="D46">
+        <v>0.3</v>
+      </c>
+      <c r="E46">
+        <v>0.05624297918743041</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47">
+        <v>396.708994174616</v>
+      </c>
+      <c r="D47">
+        <v>0.3</v>
+      </c>
+      <c r="E47">
+        <v>0.05261392495684562</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" t="s">
+        <v>138</v>
+      </c>
+      <c r="C48">
+        <v>177.6992560488625</v>
+      </c>
+      <c r="D48">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E48">
+        <v>0.06417452367239529</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" t="s">
+        <v>139</v>
+      </c>
+      <c r="C49">
+        <v>682.2350483073744</v>
+      </c>
+      <c r="D49">
+        <v>0.3</v>
+      </c>
+      <c r="E49">
+        <v>0.08875179501852146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" t="s">
+        <v>140</v>
+      </c>
+      <c r="C50">
+        <v>602.0588764809884</v>
+      </c>
+      <c r="D50">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E50">
+        <v>0.06340799120389556</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" t="s">
+        <v>141</v>
+      </c>
+      <c r="C51">
+        <v>1208.777626889244</v>
+      </c>
+      <c r="D51">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E51">
+        <v>0.06295388921875132</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" t="s">
+        <v>142</v>
+      </c>
+      <c r="C52">
+        <v>800.8551332905564</v>
+      </c>
+      <c r="D52">
+        <v>0.3</v>
+      </c>
+      <c r="E52">
+        <v>0.06244971407443516</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" t="s">
+        <v>143</v>
+      </c>
+      <c r="C53">
+        <v>550.5864214181979</v>
+      </c>
+      <c r="D53">
+        <v>0.3</v>
+      </c>
+      <c r="E53">
+        <v>0.06988911162962655</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54" t="s">
+        <v>144</v>
+      </c>
+      <c r="C54">
+        <v>329.7169742633172</v>
+      </c>
+      <c r="D54">
+        <v>0.3</v>
+      </c>
+      <c r="E54">
+        <v>0.0541585043139483</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" t="s">
+        <v>145</v>
+      </c>
+      <c r="C55">
+        <v>1565.407741369039</v>
+      </c>
+      <c r="D55">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E55">
+        <v>0.06375627179444625</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" t="s">
+        <v>146</v>
+      </c>
+      <c r="C56">
+        <v>594.6235457991907</v>
+      </c>
+      <c r="D56">
+        <v>0.3</v>
+      </c>
+      <c r="E56">
+        <v>0.06825339139109167</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" t="s">
+        <v>147</v>
+      </c>
+      <c r="C57">
+        <v>905.9282679681766</v>
+      </c>
+      <c r="D57">
+        <v>0.3</v>
+      </c>
+      <c r="E57">
+        <v>0.06190994792374609</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" t="s">
+        <v>148</v>
+      </c>
+      <c r="C58">
+        <v>302.9514503856519</v>
+      </c>
+      <c r="D58">
+        <v>0.3</v>
+      </c>
+      <c r="E58">
+        <v>0.06686194005421582</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" t="s">
+        <v>149</v>
+      </c>
+      <c r="C59">
+        <v>1375.697023803415</v>
+      </c>
+      <c r="D59">
+        <v>0.3</v>
+      </c>
+      <c r="E59">
+        <v>0.1048309855828252</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60">
+        <v>578.5126357005744</v>
+      </c>
+      <c r="D60">
+        <v>0.3</v>
+      </c>
+      <c r="E60">
+        <v>0.0682691333137331</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B61" t="s">
+        <v>151</v>
+      </c>
+      <c r="C61">
+        <v>920.9375175289357</v>
+      </c>
+      <c r="D61">
+        <v>0.3</v>
+      </c>
+      <c r="E61">
+        <v>0.07882039691278121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62" t="s">
+        <v>152</v>
+      </c>
+      <c r="C62">
+        <v>473.9751504631852</v>
+      </c>
+      <c r="D62">
+        <v>0.3</v>
+      </c>
+      <c r="E62">
+        <v>0.06757558461123257</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" t="s">
+        <v>153</v>
+      </c>
+      <c r="C63">
+        <v>490.0657728079262</v>
+      </c>
+      <c r="D63">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E63">
+        <v>0.09082019510895593</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" t="s">
+        <v>154</v>
+      </c>
+      <c r="C64">
+        <v>307.5921787162156</v>
+      </c>
+      <c r="D64">
+        <v>0.3</v>
+      </c>
+      <c r="E64">
+        <v>0.0930405864235377</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" t="s">
+        <v>155</v>
+      </c>
+      <c r="C65">
+        <v>1704.624898068311</v>
+      </c>
+      <c r="D65">
+        <v>0.3</v>
+      </c>
+      <c r="E65">
+        <v>0.07483317520823177</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" t="s">
+        <v>156</v>
+      </c>
+      <c r="C66">
+        <v>404.3540994797295</v>
+      </c>
+      <c r="D66">
+        <v>0.3</v>
+      </c>
+      <c r="E66">
+        <v>0.07650976338310871</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" t="s">
+        <v>157</v>
+      </c>
+      <c r="C67">
+        <v>886.8515171581267</v>
+      </c>
+      <c r="D67">
+        <v>0.3</v>
+      </c>
+      <c r="E67">
+        <v>0.05352151582125086</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68" t="s">
+        <v>158</v>
+      </c>
+      <c r="C68">
+        <v>1505.1492997304</v>
+      </c>
+      <c r="D68">
+        <v>0.3</v>
+      </c>
+      <c r="E68">
+        <v>0.05781697459879383</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" t="s">
+        <v>159</v>
+      </c>
+      <c r="C69">
+        <v>939.798945015772</v>
+      </c>
+      <c r="D69">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E69">
+        <v>0.08572461415814758</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70" t="s">
+        <v>160</v>
+      </c>
+      <c r="C70">
+        <v>2647.504007791044</v>
+      </c>
+      <c r="D70">
+        <v>0.3</v>
+      </c>
+      <c r="E70">
+        <v>0.06323454685657411</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" t="s">
+        <v>161</v>
+      </c>
+      <c r="C71">
+        <v>313.7797239284938</v>
+      </c>
+      <c r="D71">
+        <v>0.3</v>
+      </c>
+      <c r="E71">
+        <v>0.05332762133387046</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>75</v>
+      </c>
+      <c r="B72" t="s">
+        <v>162</v>
+      </c>
+      <c r="C72">
+        <v>64.91167408484395</v>
+      </c>
+      <c r="D72">
+        <v>0.3</v>
+      </c>
+      <c r="E72">
+        <v>0.06536925889712382</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>76</v>
+      </c>
+      <c r="B73" t="s">
+        <v>163</v>
+      </c>
+      <c r="C73">
+        <v>53.57064232089613</v>
+      </c>
+      <c r="D73">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E73">
+        <v>0.05899850475869618</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74" t="s">
+        <v>164</v>
+      </c>
+      <c r="C74">
+        <v>78.56807063496755</v>
+      </c>
+      <c r="D74">
+        <v>0.3</v>
+      </c>
+      <c r="E74">
+        <v>0.06596815334590055</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>78</v>
+      </c>
+      <c r="B75" t="s">
+        <v>165</v>
+      </c>
+      <c r="C75">
+        <v>23.72904097965595</v>
+      </c>
+      <c r="D75">
+        <v>0.3</v>
+      </c>
+      <c r="E75">
+        <v>0.06536925889712382</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76" t="s">
+        <v>166</v>
+      </c>
+      <c r="C76">
+        <v>3.726047757136057</v>
+      </c>
+      <c r="D76">
+        <v>0.3</v>
+      </c>
+      <c r="E76">
+        <v>0.06536925889712381</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" t="s">
+        <v>167</v>
+      </c>
+      <c r="C77">
+        <v>236.2103005408986</v>
+      </c>
+      <c r="D77">
+        <v>0.3</v>
+      </c>
+      <c r="E77">
+        <v>0.09455976803078406</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78" t="s">
+        <v>168</v>
+      </c>
+      <c r="C78">
+        <v>47.26385555174958</v>
+      </c>
+      <c r="D78">
+        <v>0.3</v>
+      </c>
+      <c r="E78">
+        <v>0.06439217377622558</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>82</v>
+      </c>
+      <c r="B79" t="s">
+        <v>169</v>
+      </c>
+      <c r="C79">
+        <v>792.1290929335046</v>
+      </c>
+      <c r="D79">
+        <v>0.3</v>
+      </c>
+      <c r="E79">
+        <v>0.05922460507914053</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>83</v>
+      </c>
+      <c r="B80" t="s">
+        <v>170</v>
+      </c>
+      <c r="C80">
+        <v>80.50909707054494</v>
+      </c>
+      <c r="D80">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E80">
+        <v>0.06875243131558065</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>84</v>
+      </c>
+      <c r="B81" t="s">
+        <v>171</v>
+      </c>
+      <c r="C81">
+        <v>75.45474883756356</v>
+      </c>
+      <c r="D81">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E81">
+        <v>0.05890300455703634</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82" t="s">
+        <v>172</v>
+      </c>
+      <c r="C82">
+        <v>428.0835630738745</v>
+      </c>
+      <c r="D82">
+        <v>0.3</v>
+      </c>
+      <c r="E82">
+        <v>0.06297198633037283</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83" t="s">
+        <v>173</v>
+      </c>
+      <c r="C83">
+        <v>174.291592217852</v>
+      </c>
+      <c r="D83">
+        <v>0.3</v>
+      </c>
+      <c r="E83">
+        <v>0.0671126654670204</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" t="s">
+        <v>174</v>
+      </c>
+      <c r="C84">
+        <v>155.0102027654304</v>
+      </c>
+      <c r="D84">
+        <v>0.3</v>
+      </c>
+      <c r="E84">
+        <v>0.08179957929574162</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>88</v>
+      </c>
+      <c r="B85" t="s">
+        <v>175</v>
+      </c>
+      <c r="C85">
+        <v>50.47281390518645</v>
+      </c>
+      <c r="D85">
+        <v>0.3</v>
+      </c>
+      <c r="E85">
+        <v>0.06615047693995603</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>89</v>
+      </c>
+      <c r="B86" t="s">
+        <v>176</v>
+      </c>
+      <c r="C86">
+        <v>119.2026560787126</v>
+      </c>
+      <c r="D86">
+        <v>0.3</v>
+      </c>
+      <c r="E86">
+        <v>0.08010931188085524</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>90</v>
+      </c>
+      <c r="B87" t="s">
+        <v>177</v>
+      </c>
+      <c r="C87">
+        <v>281.4677299644492</v>
+      </c>
+      <c r="D87">
+        <v>0.3</v>
+      </c>
+      <c r="E87">
+        <v>0.05770146165732867</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>91</v>
+      </c>
+      <c r="B88" t="s">
+        <v>178</v>
+      </c>
+      <c r="C88">
+        <v>94.3524263595417</v>
+      </c>
+      <c r="D88">
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="E88">
+        <v>0.05937849361833965</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E88"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2">
         <v>266.0719393051889</v>
       </c>
       <c r="D2">

</xml_diff>